<commit_message>
added TimeTaskerVr4.vi, and Integration - King Kong 2013 v3-1.xlsx. modified Motors SetUp.xlsx, and the Flipper Control Servo.vi.
</commit_message>
<xml_diff>
--- a/ king-kong-2230-2013/Documents/Motors SetUp.xlsx
+++ b/ king-kong-2230-2013/Documents/Motors SetUp.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27660" windowHeight="11955"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>שמות</t>
   </si>
@@ -111,13 +112,142 @@
   </si>
   <si>
     <t>Feeder Servo Right</t>
+  </si>
+  <si>
+    <t>refnum name</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function </t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Left Motor</t>
+  </si>
+  <si>
+    <t>Right Motor</t>
+  </si>
+  <si>
+    <t>רכיב</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>הסבר</t>
+  </si>
+  <si>
+    <t>הנעת צד שמאל</t>
+  </si>
+  <si>
+    <t>הנעת צד ימין</t>
+  </si>
+  <si>
+    <t>מנוע ירייה ראשון (קרוב יותר לפליפר)</t>
+  </si>
+  <si>
+    <t>מנוע ירייה שני (קרוב יותר ללוע התותח)</t>
+  </si>
+  <si>
+    <t>סרבו שמאלי של הפליפר</t>
+  </si>
+  <si>
+    <t>סרבו ימני של הפליפר</t>
+  </si>
+  <si>
+    <t>מנוע העלרוד של התותח</t>
+  </si>
+  <si>
+    <t>מסוע על האיסוף</t>
+  </si>
+  <si>
+    <t>מנוע הממוקם על התותח, מעל הפליפר, ומטרתו להעביר את הפריסבי לתותח.</t>
+  </si>
+  <si>
+    <t>סרבו המתחבר לציר ה-Y המצלמה</t>
+  </si>
+  <si>
+    <t>סרבו שמאלי של הפידר</t>
+  </si>
+  <si>
+    <t>סרבו ימני של הפידר</t>
+  </si>
+  <si>
+    <t>בונד</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>InCannon</t>
+  </si>
+  <si>
+    <t>InFlipper</t>
+  </si>
+  <si>
+    <t>ג'יימס</t>
+  </si>
+  <si>
+    <t>MS בתא התחתון של האיסוף</t>
+  </si>
+  <si>
+    <t>MS בתא האמצעי של האיסוף</t>
+  </si>
+  <si>
+    <t>MS על הפליפר</t>
+  </si>
+  <si>
+    <t>MS ממוקם על הפרופיל שנמצא על התותח</t>
+  </si>
+  <si>
+    <t>zAvit Upper LS</t>
+  </si>
+  <si>
+    <t>zAvit Lower LS</t>
+  </si>
+  <si>
+    <t>Enc</t>
+  </si>
+  <si>
+    <t>CannonAI</t>
+  </si>
+  <si>
+    <t>אנקודר אופטי</t>
+  </si>
+  <si>
+    <t>אנקודר אנלוגי</t>
+  </si>
+  <si>
+    <t>אנקודר המחובר לציר המנוע של הירייה</t>
+  </si>
+  <si>
+    <t>אנקודר אנלוגי המחובר לציר התותח</t>
+  </si>
+  <si>
+    <t>limit switch - הממוקם בראש התותח</t>
+  </si>
+  <si>
+    <t>limit switch - הממוקם בתחתית התותח</t>
+  </si>
+  <si>
+    <t>מנוע סים שמחובר לגיר חלזוני כחול שמחובר ליגואר שמאל</t>
+  </si>
+  <si>
+    <t>מנוע סים שמחובר לגיר חלזוני כחול שמחובר ליגואר ימין</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +266,13 @@
       <b/>
       <i/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -174,12 +311,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -194,12 +346,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -219,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -507,11 +680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.125" customWidth="1"/>
     <col min="2" max="3" width="10.625" customWidth="1"/>
@@ -533,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -567,7 +740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -601,7 +774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -615,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -629,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -643,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -657,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -671,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -685,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -699,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -713,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -727,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -741,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -755,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -769,7 +942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -783,7 +956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -797,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -818,4 +991,533 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="8">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="8">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>